<commit_message>
updated scenarios to include wdc and cpCable booleans
</commit_message>
<xml_diff>
--- a/sites/packing-for-peanuts/Small Shipper.xlsx
+++ b/sites/packing-for-peanuts/Small Shipper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Level 1 Access\WAREHOUSE DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesselafica/sites/shs/sites/packing-for-peanuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210F18E3-F068-4F64-B9B1-EE9989B9CCBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAD6CAC-AD9F-AD49-920F-1BDA0AC77F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55E280F1-9D35-42A7-9588-1C8256B3190D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{55E280F1-9D35-42A7-9588-1C8256B3190D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>API</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
   </si>
   <si>
     <t>Scenario 13</t>
-  </si>
-  <si>
-    <t>N/a</t>
   </si>
   <si>
     <t>Scenario 14</t>
@@ -634,25 +628,25 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -681,10 +675,10 @@
         <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -713,10 +707,10 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -745,10 +739,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -777,10 +771,10 @@
         <v>18</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -809,10 +803,10 @@
         <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -841,10 +835,10 @@
         <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -870,13 +864,13 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -902,13 +896,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -937,10 +931,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -969,77 +963,77 @@
         <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
@@ -1056,44 +1050,44 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1123,9 +1117,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1155,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,18 +1157,18 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
@@ -1192,14 +1186,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1214,17 +1208,17 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
@@ -1239,17 +1233,17 @@
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -1264,17 +1258,17 @@
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1289,17 +1283,17 @@
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
@@ -1314,17 +1308,17 @@
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1">
         <v>5</v>
@@ -1339,17 +1333,17 @@
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1364,67 +1358,67 @@
         <v>2</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="1">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1">
-        <v>18</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
-      <c r="E40" s="1">
-        <v>1</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1439,42 +1433,42 @@
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="1">
-        <v>2</v>
-      </c>
-      <c r="E44" s="1">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="B46" s="1">
         <v>2</v>
@@ -1489,42 +1483,42 @@
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B48" s="1">
-        <v>2</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="B50" s="1">
         <v>3</v>
@@ -1542,95 +1536,95 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="1">
-        <v>0</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B56" s="1">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="1">
-        <v>2</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="D56" s="1">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B56" s="1">
-        <v>2</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2</v>
-      </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B58" s="1">
         <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58" s="1">
         <v>2</v>
@@ -1642,20 +1636,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1">
         <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="1">
         <v>2</v>
@@ -1664,23 +1658,23 @@
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="1">
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62" s="1">
         <v>2</v>

</xml_diff>